<commit_message>
chore: clean up empty code change sections in the changes log
</commit_message>
<xml_diff>
--- a/InputList/FullBand/InputList.xlsx
+++ b/InputList/FullBand/InputList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\TechnicalDocumentation\Input List\FullBand\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\InputList\FullBand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{4CEF91C4-2EFC-4BF5-9621-AFEB67DBAD9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EC463F-B33F-49FE-9943-A03ECF7582EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="38280" yWindow="-7425" windowWidth="16440" windowHeight="29040" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Channels" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,6 @@
     <definedName name="Stand">Channels!$H$4:$H$33</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -588,54 +587,6 @@
     <t>D10</t>
   </si>
   <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>B3</t>
-  </si>
-  <si>
-    <t>B4</t>
-  </si>
-  <si>
-    <t>B5</t>
-  </si>
-  <si>
-    <t>B6</t>
-  </si>
-  <si>
-    <t>B7</t>
-  </si>
-  <si>
-    <t>B8</t>
-  </si>
-  <si>
-    <t>B9</t>
-  </si>
-  <si>
-    <t>B10</t>
-  </si>
-  <si>
-    <t>B11</t>
-  </si>
-  <si>
-    <t>B12</t>
-  </si>
-  <si>
-    <t>B13</t>
-  </si>
-  <si>
-    <t>B14</t>
-  </si>
-  <si>
-    <t>B15</t>
-  </si>
-  <si>
-    <t>B16</t>
-  </si>
-  <si>
     <t>USR 2</t>
   </si>
   <si>
@@ -661,6 +612,54 @@
   <si>
     <t>Kenzi
 Acstc</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>A16</t>
   </si>
 </sst>
 </file>
@@ -1197,11 +1196,17 @@
     <xf numFmtId="0" fontId="20" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1217,23 +1222,17 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1759,55 +1758,55 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.81640625" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" customWidth="1"/>
-    <col min="11" max="13" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.81640625" customWidth="1"/>
+    <col min="11" max="13" width="7.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="e" vm="1">
+    <row r="1" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="47" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="47" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
       <c r="I1" s="8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
+    <row r="2" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
       <c r="I2" s="9" t="str">
         <f ca="1">"Date Updated: "&amp;TEXT(TODAY(),"yyyy.mm.dd")</f>
-        <v>Date Updated: 2026.02.08</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>Date Updated: 2026.02.11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>37</v>
       </c>
@@ -1836,11 +1835,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
+    <row r="4" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="53" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="15">
@@ -1865,9 +1864,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="49"/>
-      <c r="B5" s="50"/>
+    <row r="5" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
       <c r="C5" s="17">
         <v>2</v>
       </c>
@@ -1890,9 +1889,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
-      <c r="B6" s="50"/>
+    <row r="6" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="52"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="15">
         <v>3</v>
       </c>
@@ -1913,9 +1912,9 @@
       </c>
       <c r="I6" s="16"/>
     </row>
-    <row r="7" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
-      <c r="B7" s="50"/>
+    <row r="7" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="52"/>
+      <c r="B7" s="53"/>
       <c r="C7" s="17">
         <v>4</v>
       </c>
@@ -1938,9 +1937,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
-      <c r="B8" s="50"/>
+    <row r="8" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="52"/>
+      <c r="B8" s="53"/>
       <c r="C8" s="15">
         <v>5</v>
       </c>
@@ -1963,9 +1962,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
-      <c r="B9" s="50"/>
+    <row r="9" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="52"/>
+      <c r="B9" s="53"/>
       <c r="C9" s="17">
         <v>6</v>
       </c>
@@ -1988,9 +1987,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
-      <c r="B10" s="50"/>
+    <row r="10" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="52"/>
+      <c r="B10" s="53"/>
       <c r="C10" s="15">
         <v>7</v>
       </c>
@@ -2013,9 +2012,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="50"/>
+    <row r="11" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="52"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="17">
         <v>8</v>
       </c>
@@ -2038,9 +2037,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="50"/>
+    <row r="12" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="52"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="15">
         <v>9</v>
       </c>
@@ -2063,9 +2062,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="B13" s="50"/>
+    <row r="13" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="52"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="17">
         <v>10</v>
       </c>
@@ -2088,7 +2087,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="19">
@@ -2096,14 +2095,14 @@
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
-      <c r="F14" s="43" t="s">
+      <c r="F14" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-    </row>
-    <row r="15" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
+    </row>
+    <row r="15" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="19">
@@ -2111,14 +2110,14 @@
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
-      <c r="F15" s="43" t="s">
+      <c r="F15" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
-    </row>
-    <row r="16" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+    </row>
+    <row r="16" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="19">
@@ -2126,25 +2125,25 @@
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
-      <c r="F16" s="43" t="s">
+      <c r="F16" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
-    </row>
-    <row r="17" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="51" t="s">
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
+    </row>
+    <row r="17" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="44" t="s">
         <v>133</v>
       </c>
       <c r="C17" s="21">
         <v>14</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="22" t="s">
@@ -2160,17 +2159,17 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
-      <c r="B18" s="52"/>
+    <row r="18" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="43"/>
+      <c r="B18" s="44"/>
       <c r="C18" s="23">
         <v>15</v>
       </c>
       <c r="D18" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="E18" s="24" t="s">
         <v>163</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>179</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>102</v>
@@ -2183,7 +2182,7 @@
       </c>
       <c r="I18" s="24"/>
     </row>
-    <row r="19" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="19">
@@ -2191,14 +2190,14 @@
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
-      <c r="F19" s="43" t="s">
+      <c r="F19" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-    </row>
-    <row r="20" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+    </row>
+    <row r="20" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="42" t="s">
         <v>57</v>
       </c>
@@ -2209,7 +2208,7 @@
         <v>17</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>75</v>
@@ -2227,21 +2226,21 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53" t="s">
+    <row r="21" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="45" t="s">
         <v>134</v>
       </c>
       <c r="C21" s="26">
         <v>18</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="F21" s="27" t="s">
         <v>1</v>
@@ -2256,14 +2255,14 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
-      <c r="B22" s="53"/>
+    <row r="22" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="45"/>
+      <c r="B22" s="45"/>
       <c r="C22" s="28">
         <v>19</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="E22" s="29" t="s">
         <v>26</v>
@@ -2279,14 +2278,14 @@
       </c>
       <c r="I22" s="29"/>
     </row>
-    <row r="23" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
-      <c r="B23" s="53"/>
+    <row r="23" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="45"/>
+      <c r="B23" s="45"/>
       <c r="C23" s="26">
         <v>20</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="E23" s="27" t="s">
         <v>26</v>
@@ -2302,14 +2301,14 @@
       </c>
       <c r="I23" s="27"/>
     </row>
-    <row r="24" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
-      <c r="B24" s="53"/>
+    <row r="24" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="45"/>
+      <c r="B24" s="45"/>
       <c r="C24" s="28">
         <v>21</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="E24" s="29" t="s">
         <v>77</v>
@@ -2325,7 +2324,7 @@
       </c>
       <c r="I24" s="29"/>
     </row>
-    <row r="25" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="19">
@@ -2333,31 +2332,31 @@
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
-      <c r="F25" s="43" t="s">
+      <c r="F25" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="G25" s="43" t="s">
+      <c r="G25" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="H25" s="43" t="s">
+      <c r="H25" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="I25" s="43" t="s">
+      <c r="I25" s="51" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="54" t="s">
+    <row r="26" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="46" t="s">
         <v>142</v>
       </c>
       <c r="C26" s="37">
         <v>23</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="E26" s="38" t="s">
         <v>76</v>
@@ -2375,17 +2374,17 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
-      <c r="B27" s="54"/>
+    <row r="27" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="46"/>
+      <c r="B27" s="46"/>
       <c r="C27" s="39">
         <v>24</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="E27" s="40" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="F27" s="40" t="s">
         <v>150</v>
@@ -2398,17 +2397,17 @@
       </c>
       <c r="I27" s="40"/>
     </row>
-    <row r="28" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="54"/>
-      <c r="B28" s="54"/>
+    <row r="28" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="46"/>
+      <c r="B28" s="46"/>
       <c r="C28" s="37">
         <v>25</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="E28" s="38" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="F28" s="38" t="s">
         <v>151</v>
@@ -2421,14 +2420,14 @@
       </c>
       <c r="I28" s="38"/>
     </row>
-    <row r="29" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
-      <c r="B29" s="54"/>
+    <row r="29" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="46"/>
+      <c r="B29" s="46"/>
       <c r="C29" s="39">
         <v>26</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="E29" s="40" t="s">
         <v>131</v>
@@ -2444,7 +2443,7 @@
       </c>
       <c r="I29" s="40"/>
     </row>
-    <row r="30" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="55" t="s">
         <v>59</v>
       </c>
@@ -2455,7 +2454,7 @@
         <v>27</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="E30" s="30" t="s">
         <v>78</v>
@@ -2473,14 +2472,14 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="55"/>
       <c r="B31" s="56"/>
       <c r="C31" s="31">
         <v>28</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="E31" s="31" t="s">
         <v>79</v>
@@ -2496,14 +2495,14 @@
       </c>
       <c r="I31" s="31"/>
     </row>
-    <row r="32" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="55"/>
       <c r="B32" s="56"/>
       <c r="C32" s="30">
         <v>29</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="E32" s="30" t="s">
         <v>80</v>
@@ -2519,17 +2518,17 @@
       </c>
       <c r="I32" s="30"/>
     </row>
-    <row r="33" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="55"/>
       <c r="B33" s="56"/>
       <c r="C33" s="31">
         <v>30</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="E33" s="31" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="F33" s="31" t="s">
         <v>32</v>
@@ -2542,7 +2541,7 @@
       </c>
       <c r="I33" s="31"/>
     </row>
-    <row r="34" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="19">
@@ -2550,12 +2549,12 @@
       </c>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-    </row>
-    <row r="35" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="51"/>
+    </row>
+    <row r="35" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="34" t="s">
         <v>127</v>
       </c>
@@ -2566,7 +2565,7 @@
         <v>32</v>
       </c>
       <c r="D35" s="36" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="E35" s="36"/>
       <c r="F35" s="36" t="s">
@@ -2582,8 +2581,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="44" t="s">
+    <row r="36" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="54" t="s">
         <v>47</v>
       </c>
       <c r="B36" s="11" t="s">
@@ -2609,68 +2608,68 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
+    <row r="37" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="54"/>
       <c r="B37" s="41"/>
       <c r="C37" s="19">
         <v>34</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="20"/>
-      <c r="F37" s="43" t="s">
+      <c r="F37" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-    </row>
-    <row r="38" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="44"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="51"/>
+    </row>
+    <row r="38" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="54"/>
       <c r="B38" s="41"/>
       <c r="C38" s="19">
         <v>35</v>
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
-      <c r="F38" s="43" t="s">
+      <c r="F38" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-    </row>
-    <row r="39" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="51"/>
+      <c r="I38" s="51"/>
+    </row>
+    <row r="39" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="54"/>
       <c r="B39" s="41"/>
       <c r="C39" s="19">
         <v>36</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="20"/>
-      <c r="F39" s="43" t="s">
+      <c r="F39" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="43"/>
-    </row>
-    <row r="40" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="44"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+    </row>
+    <row r="40" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="54"/>
       <c r="B40" s="41"/>
       <c r="C40" s="19">
         <v>37</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="20"/>
-      <c r="F40" s="43" t="s">
+      <c r="F40" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="G40" s="43"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="43"/>
-    </row>
-    <row r="41" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="44"/>
+      <c r="G40" s="51"/>
+      <c r="H40" s="51"/>
+      <c r="I40" s="51"/>
+    </row>
+    <row r="41" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="54"/>
       <c r="B41" s="11" t="s">
         <v>28</v>
       </c>
@@ -2692,23 +2691,23 @@
       </c>
       <c r="I41" s="33"/>
     </row>
-    <row r="42" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="44"/>
+    <row r="42" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="54"/>
       <c r="B42" s="41"/>
       <c r="C42" s="19">
         <v>39</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="20"/>
-      <c r="F42" s="43" t="s">
+      <c r="F42" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="G42" s="43"/>
-      <c r="H42" s="43"/>
-      <c r="I42" s="43"/>
-    </row>
-    <row r="43" spans="1:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="44"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="51"/>
+      <c r="I42" s="51"/>
+    </row>
+    <row r="43" spans="1:9" ht="11.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="54"/>
       <c r="B43" s="11" t="s">
         <v>104</v>
       </c>
@@ -2732,17 +2731,17 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
     <mergeCell ref="F25:I25"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="F37:I37"/>
     <mergeCell ref="F40:I40"/>
     <mergeCell ref="A36:A43"/>
     <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:H2"/>
     <mergeCell ref="F15:I15"/>
@@ -2771,32 +2770,32 @@
       <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="8" width="8.7109375" customWidth="1"/>
+    <col min="1" max="8" width="8.7265625" customWidth="1"/>
     <col min="9" max="10" width="2" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="e" vm="1">
+    <row r="1" spans="1:16" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="47" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="47" t="str">
+      <c r="B1" s="47"/>
+      <c r="C1" s="49" t="str">
         <f>Channels!C1</f>
         <v>Full Band Setup</v>
       </c>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="81" t="str">
         <f>Channels!I1</f>
         <v>🌐 theperfectstrangers.band</v>
@@ -2807,25 +2806,25 @@
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
     </row>
-    <row r="2" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
+    <row r="2" spans="1:16" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
       <c r="K2" s="84" t="str">
         <f ca="1">Channels!I2</f>
-        <v>Date Updated: 2026.02.08</v>
+        <v>Date Updated: 2026.02.11</v>
       </c>
       <c r="L2" s="84"/>
       <c r="M2" s="84"/>
     </row>
-    <row r="3" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>105</v>
       </c>
@@ -2843,7 +2842,7 @@
       <c r="L3" s="68"/>
       <c r="M3" s="68"/>
     </row>
-    <row r="4" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="63" t="s">
         <v>0</v>
       </c>
@@ -2863,7 +2862,7 @@
       </c>
       <c r="M4" s="70"/>
     </row>
-    <row r="5" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -2893,7 +2892,7 @@
       <c r="L5" s="71"/>
       <c r="M5" s="72"/>
     </row>
-    <row r="6" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="83" t="s">
         <v>12</v>
       </c>
@@ -2927,7 +2926,7 @@
       </c>
       <c r="M6" s="74"/>
     </row>
-    <row r="7" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="83"/>
       <c r="B7" s="83"/>
       <c r="C7" s="83"/>
@@ -2941,7 +2940,7 @@
       <c r="L7" s="75"/>
       <c r="M7" s="76"/>
     </row>
-    <row r="8" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -2959,7 +2958,7 @@
       </c>
       <c r="M8" s="70"/>
     </row>
-    <row r="9" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>9</v>
       </c>
@@ -2989,7 +2988,7 @@
       <c r="L9" s="71"/>
       <c r="M9" s="72"/>
     </row>
-    <row r="10" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="85" t="s">
         <v>42</v>
       </c>
@@ -3011,7 +3010,7 @@
       </c>
       <c r="M10" s="74"/>
     </row>
-    <row r="11" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="86"/>
       <c r="B11" s="83"/>
       <c r="C11" s="57"/>
@@ -3025,7 +3024,7 @@
       <c r="L11" s="75"/>
       <c r="M11" s="76"/>
     </row>
-    <row r="12" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="I12" s="2"/>
       <c r="K12" s="79">
         <v>5</v>
@@ -3035,7 +3034,7 @@
       </c>
       <c r="M12" s="70"/>
     </row>
-    <row r="13" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>17</v>
       </c>
@@ -3065,7 +3064,7 @@
       <c r="L13" s="71"/>
       <c r="M13" s="72"/>
     </row>
-    <row r="14" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="58" t="s">
         <v>115</v>
       </c>
@@ -3091,7 +3090,7 @@
       <c r="L14" s="73"/>
       <c r="M14" s="74"/>
     </row>
-    <row r="15" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="58"/>
       <c r="B15" s="58"/>
       <c r="C15" s="57"/>
@@ -3105,10 +3104,10 @@
       <c r="L15" s="75"/>
       <c r="M15" s="76"/>
     </row>
-    <row r="16" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:13" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="14.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="63" t="s">
         <v>4</v>
       </c>
@@ -3121,7 +3120,7 @@
       <c r="H17" s="63"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:13" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="14.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -3153,7 +3152,7 @@
       <c r="L18" s="67"/>
       <c r="M18" s="67"/>
     </row>
-    <row r="19" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="61" t="s">
         <v>108</v>
       </c>
@@ -3189,7 +3188,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="61"/>
       <c r="B20" s="61"/>
       <c r="C20" s="62"/>
@@ -3209,7 +3208,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="14.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -3229,7 +3228,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="14.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="I22" s="2"/>
       <c r="K22" t="s">
         <v>93</v>
@@ -3241,7 +3240,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="63" t="s">
         <v>106</v>
       </c>
@@ -3263,7 +3262,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="63" t="s">
         <v>0</v>
       </c>
@@ -3285,7 +3284,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -3321,7 +3320,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="65" t="s">
         <v>98</v>
       </c>
@@ -3348,7 +3347,7 @@
       </c>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="66"/>
       <c r="B27" s="61"/>
       <c r="C27" s="62"/>
@@ -3359,7 +3358,7 @@
       <c r="H27" s="87"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -3370,7 +3369,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>9</v>
       </c>
@@ -3397,12 +3396,12 @@
       </c>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="87" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="B30" s="87" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="C30" s="88" t="s">
         <v>138</v>
@@ -3417,14 +3416,14 @@
         <v>59</v>
       </c>
       <c r="G30" s="90" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="H30" s="92" t="s">
         <v>147</v>
       </c>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="87"/>
       <c r="B31" s="87"/>
       <c r="C31" s="89"/>
@@ -3435,10 +3434,10 @@
       <c r="H31" s="92"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="63" t="s">
         <v>4</v>
       </c>
@@ -3451,7 +3450,7 @@
       <c r="H33" s="63"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>1</v>
       </c>
@@ -3478,7 +3477,7 @@
       </c>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="83" t="s">
         <v>112</v>
       </c>
@@ -3505,7 +3504,7 @@
       </c>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="83"/>
       <c r="B36" s="83"/>
       <c r="C36" s="87"/>

</xml_diff>